<commit_message>
RITM0167688 - [RPA] Capy FIN009 Migration for Project Catalyst
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a9005130_adm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessica.lara\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7A8A0E-3F44-4AFD-9885-AB60A975648E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -389,14 +390,14 @@
     <t>Data/Output/</t>
   </si>
   <si>
-    <t>https://launchpad.orica.net/fiori#Shell-home</t>
+    <t>https://launchpad-dt.orica.net/fiori#Shell-home</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -420,6 +421,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -438,31 +445,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -773,7 +780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -881,9 +888,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B10" s="5"/>
-    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1880,11 +1885,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2085,7 +2090,7 @@
         <v>51</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
@@ -2109,7 +2114,7 @@
       <c r="A28" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="7" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2117,7 +2122,7 @@
       <c r="A29" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2125,7 +2130,7 @@
       <c r="A30" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2133,7 +2138,7 @@
       <c r="A31" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="2" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2149,7 +2154,7 @@
       <c r="A33" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2157,7 +2162,7 @@
       <c r="A34" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="5" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2323,7 +2328,7 @@
       <c r="A60" t="s">
         <v>111</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="6" t="s">
         <v>112</v>
       </c>
       <c r="C60" t="s">
@@ -3281,13 +3286,16 @@
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B28" r:id="rId1" location="Shell-home" xr:uid="{BEFEDCED-E844-4D82-B851-4BBDB6716B7B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>